<commit_message>
Added indavidual functions for each branch
</commit_message>
<xml_diff>
--- a/member_list.xlsx
+++ b/member_list.xlsx
@@ -1,14 +1,22 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="27108"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="4" rupBuild="26924"/>
   <workbookPr defaultThemeVersion="166925"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{686F3861-A289-4A71-B8BB-0F9DD9CA4585}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice Requires="x15">
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\bmt81\Documents\Personal Projects\SGA-Discord-Bot\"/>
+    </mc:Choice>
+  </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD57F1B5-E880-435A-AA46-87420DB20C31}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="105" windowWidth="14805" windowHeight="8010" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="executive_board" sheetId="1" r:id="rId1"/>
+    <sheet name="executive_cabinet" sheetId="5" r:id="rId2"/>
+    <sheet name="legislative" sheetId="2" r:id="rId3"/>
+    <sheet name="judicial" sheetId="3" r:id="rId4"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -31,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6" uniqueCount="6">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="66" uniqueCount="49">
   <si>
     <t>Brandon Townes</t>
   </si>
@@ -39,26 +47,162 @@
     <t>Florida PolyCon President</t>
   </si>
   <si>
-    <t>Senior</t>
-  </si>
-  <si>
-    <t>Alis Craig</t>
-  </si>
-  <si>
-    <t>Director of NOVA</t>
-  </si>
-  <si>
-    <t>Sophmore</t>
+    <t>Student Body President</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Position</t>
+  </si>
+  <si>
+    <t>Off-Campus Representative</t>
+  </si>
+  <si>
+    <t>On-Campus Representative</t>
+  </si>
+  <si>
+    <t>Chief Justice</t>
+  </si>
+  <si>
+    <t>Senior Representative</t>
+  </si>
+  <si>
+    <t>Associate Justice</t>
+  </si>
+  <si>
+    <t>Engineering Representative</t>
+  </si>
+  <si>
+    <t>Technology Representative</t>
+  </si>
+  <si>
+    <t>Sophomore Representative</t>
+  </si>
+  <si>
+    <t>Freshman Representative</t>
+  </si>
+  <si>
+    <t>Director of Student Media</t>
+  </si>
+  <si>
+    <t>Student Body Treasurer</t>
+  </si>
+  <si>
+    <t>Chief of Staff</t>
+  </si>
+  <si>
+    <t>Sustainability President</t>
+  </si>
+  <si>
+    <t>Director of Internal Affairs</t>
+  </si>
+  <si>
+    <t>Deputy of Communications</t>
+  </si>
+  <si>
+    <t>Student Body Vice President</t>
+  </si>
+  <si>
+    <t>Director of External Affairs</t>
+  </si>
+  <si>
+    <t>John Paul Jones</t>
+  </si>
+  <si>
+    <t>Madeleine Prewett</t>
+  </si>
+  <si>
+    <t>Johanna Campbell</t>
+  </si>
+  <si>
+    <t>Brian Curci</t>
+  </si>
+  <si>
+    <t>Jacob Brescia</t>
+  </si>
+  <si>
+    <t>Trent Halama</t>
+  </si>
+  <si>
+    <t>Clayton Dodd</t>
+  </si>
+  <si>
+    <t>Jacqileen Custer</t>
+  </si>
+  <si>
+    <t>Kaydence Johnson</t>
+  </si>
+  <si>
+    <t>Melissa Fayo Guzman</t>
+  </si>
+  <si>
+    <t>Angel Moreta</t>
+  </si>
+  <si>
+    <t>Christopher Bruckner</t>
+  </si>
+  <si>
+    <t>Brian Tran</t>
+  </si>
+  <si>
+    <t>Wilson Hendershot</t>
+  </si>
+  <si>
+    <t>Charles Sirjue</t>
+  </si>
+  <si>
+    <t>Liana Nazario</t>
+  </si>
+  <si>
+    <t>Georgette Amancha</t>
+  </si>
+  <si>
+    <t>Jaylyn Leatherwood</t>
+  </si>
+  <si>
+    <t>Colby Manrodt</t>
+  </si>
+  <si>
+    <t>Elizabeth Spurlock</t>
+  </si>
+  <si>
+    <t>Lang Towl</t>
+  </si>
+  <si>
+    <t>Melia Rodriguez</t>
+  </si>
+  <si>
+    <t>Cole Rhodes</t>
+  </si>
+  <si>
+    <t>Dimitri Tsetsekas</t>
+  </si>
+  <si>
+    <t>Taki Tsetsekas</t>
+  </si>
+  <si>
+    <t>Ranking Justice</t>
+  </si>
+  <si>
+    <t>Jonathan Gauthier</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -72,7 +216,7 @@
       <patternFill patternType="gray125"/>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -80,12 +224,53 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </right>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="1">
+  <cellXfs count="6">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -101,6 +286,50 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{5712D2DC-2C6F-430F-B39D-5082B93347DD}" name="Table1" displayName="Table1" ref="A1:B5" totalsRowShown="0">
+  <autoFilter ref="A1:B5" xr:uid="{5712D2DC-2C6F-430F-B39D-5082B93347DD}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{5DF6A680-EB24-49F8-970D-49D30E177BE6}" name="Position"/>
+    <tableColumn id="2" xr3:uid="{648DFC42-ABF1-4E5D-B866-31229BF02E3C}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{E7CE413C-F498-497C-8F23-A08184FDECBF}" name="Table15" displayName="Table15" ref="A1:B7" totalsRowShown="0">
+  <autoFilter ref="A1:B7" xr:uid="{E7CE413C-F498-497C-8F23-A08184FDECBF}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{821CA441-2133-42BA-A8A3-27BD76AC74D2}" name="Position"/>
+    <tableColumn id="2" xr3:uid="{C9381C95-AF3C-404B-8429-39EA0F937E6A}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{E0D784DA-44E9-4746-BB0B-B314365553C2}" name="Table13" displayName="Table13" ref="A1:B15" totalsRowShown="0">
+  <autoFilter ref="A1:B15" xr:uid="{E0D784DA-44E9-4746-BB0B-B314365553C2}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{D5A00315-A6BB-4552-A64C-8B9AFEBC1683}" name="Position"/>
+    <tableColumn id="2" xr3:uid="{5C6A4199-8F47-4BA7-99F3-3F64152FCAFA}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{8A4CECBB-C67D-473F-AC35-568694A8BD13}" name="Table14" displayName="Table14" ref="A1:B6" totalsRowShown="0">
+  <autoFilter ref="A1:B6" xr:uid="{8A4CECBB-C67D-473F-AC35-568694A8BD13}"/>
+  <tableColumns count="2">
+    <tableColumn id="1" xr3:uid="{9C0620D7-A100-4A17-BF0C-79A8204AC420}" name="Position"/>
+    <tableColumn id="2" xr3:uid="{4D62188E-38D2-43AE-B5F9-415B0A68A3F6}" name="Name"/>
+  </tableColumns>
+  <tableStyleInfo name="TableStyleMedium2" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -400,37 +629,352 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:C2"/>
+  <dimension ref="A1:B5"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G15" sqref="G15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="32" customWidth="1"/>
+    <col min="2" max="2" width="28" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>43</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>15</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="4" t="s">
+        <v>16</v>
+      </c>
+      <c r="B5" s="5" t="s">
+        <v>40</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{09C8523F-7FB2-4E8B-B3A2-163FF4D75A6F}">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B11" sqref="B11"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="26.44140625" customWidth="1"/>
+    <col min="2" max="2" width="24.33203125" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>41</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>18</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>19</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>21</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>46</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{3731C79F-D9F5-4E69-8F71-32490DFFAB91}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A18" sqref="A18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="30.6640625" customWidth="1"/>
+    <col min="2" max="2" width="27" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A1" t="s">
+        <v>4</v>
+      </c>
+      <c r="B1" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>5</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>6</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>8</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>29</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A7" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>31</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A8" s="1" t="s">
+        <v>11</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A9" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A10" s="1" t="s">
+        <v>12</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A11" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A12" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A13" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A14" s="1" t="s">
+        <v>14</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A15" s="1" t="s">
+        <v>10</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{6D6F6F1B-73CC-4897-9633-17A3B8A90ADB}">
+  <dimension ref="A1:B6"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D6" sqref="D6"/>
+      <selection activeCell="B8" sqref="B8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="1" width="28.21875" customWidth="1"/>
+    <col min="2" max="2" width="26.33203125" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:3">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
-        <v>0</v>
+        <v>4</v>
       </c>
       <c r="B1" t="s">
-        <v>1</v>
-      </c>
-      <c r="C1" t="s">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3">
-      <c r="A2" t="s">
         <v>3</v>
       </c>
-      <c r="B2" t="s">
-        <v>4</v>
-      </c>
-      <c r="C2" t="s">
-        <v>5</v>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A2" s="1" t="s">
+        <v>7</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>24</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A3" s="1" t="s">
+        <v>47</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A4" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A5" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A6" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>30</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId1"/>
+  </tableParts>
 </worksheet>
 </file>
</xml_diff>